<commit_message>
added rounding down to tens
</commit_message>
<xml_diff>
--- a/input/sneakers.xlsx
+++ b/input/sneakers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patryk_dratwa/Documents/codes/bestSizeChecker/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D0E3375-4745-C44B-95F2-67C2A43FC21C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48E84A01-78A9-8340-B1BA-46DB29C026DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="127">
   <si>
     <t>sku</t>
   </si>
@@ -377,6 +377,42 @@
   </si>
   <si>
     <t>DN1431-001</t>
+  </si>
+  <si>
+    <t>NI115O04G-K11</t>
+  </si>
+  <si>
+    <t>FD9749-400</t>
+  </si>
+  <si>
+    <t>NE216D05Q-A13</t>
+  </si>
+  <si>
+    <t>GSB550CA</t>
+  </si>
+  <si>
+    <t>FB1843-141</t>
+  </si>
+  <si>
+    <t>NI116D0II-T11</t>
+  </si>
+  <si>
+    <t>NI112O0GN-M11</t>
+  </si>
+  <si>
+    <t>DD1391-300</t>
+  </si>
+  <si>
+    <t>JOC11A032-M11</t>
+  </si>
+  <si>
+    <t>DR8057-500</t>
+  </si>
+  <si>
+    <t>NI112N03R-Q11</t>
+  </si>
+  <si>
+    <t>DR9512-001</t>
   </si>
 </sst>
 </file>
@@ -770,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C3ED77E-355F-451A-8EC6-B2847837F9C7}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1408,6 +1444,72 @@
       </c>
       <c r="C57" t="s">
         <v>32</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B58">
+        <v>549</v>
+      </c>
+      <c r="C58" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B59">
+        <v>339</v>
+      </c>
+      <c r="C59" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B60">
+        <v>449</v>
+      </c>
+      <c r="C60" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B61">
+        <v>499</v>
+      </c>
+      <c r="C61" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B62">
+        <v>589</v>
+      </c>
+      <c r="C62" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63">
+        <v>549</v>
+      </c>
+      <c r="C63" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>